<commit_message>
Corrections following AS review comments of today - reacquired curated summaries, removed georeference field, regenerated visualisation files, updated README files to account for mismatches and reproduction instructions, suppressed count fields in map-only visualisation, improved output from "wormify" authority checking
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Brachiopoda.xlsx
+++ b/data/dataPaper-I-in/arphified/Brachiopoda.xlsx
@@ -2700,7 +2700,7 @@
         <v>36</v>
       </c>
       <c r="CO2" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP2" t="s">
         <v>36</v>
@@ -3167,7 +3167,7 @@
         <v>36</v>
       </c>
       <c r="CO3" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP3" t="s">
         <v>36</v>
@@ -3634,7 +3634,7 @@
         <v>36</v>
       </c>
       <c r="CO4" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP4" t="s">
         <v>36</v>
@@ -4101,7 +4101,7 @@
         <v>36</v>
       </c>
       <c r="CO5" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP5" t="s">
         <v>36</v>
@@ -4568,7 +4568,7 @@
         <v>36</v>
       </c>
       <c r="CO6" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP6" t="s">
         <v>36</v>
@@ -5035,7 +5035,7 @@
         <v>36</v>
       </c>
       <c r="CO7" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP7" t="s">
         <v>36</v>
@@ -5502,7 +5502,7 @@
         <v>36</v>
       </c>
       <c r="CO8" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP8" t="s">
         <v>36</v>
@@ -5969,7 +5969,7 @@
         <v>36</v>
       </c>
       <c r="CO9" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP9" t="s">
         <v>36</v>
@@ -6436,7 +6436,7 @@
         <v>36</v>
       </c>
       <c r="CO10" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP10" t="s">
         <v>36</v>
@@ -6903,7 +6903,7 @@
         <v>36</v>
       </c>
       <c r="CO11" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP11" t="s">
         <v>36</v>
@@ -7370,7 +7370,7 @@
         <v>36</v>
       </c>
       <c r="CO12" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP12" t="s">
         <v>36</v>
@@ -7837,7 +7837,7 @@
         <v>36</v>
       </c>
       <c r="CO13" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP13" t="s">
         <v>36</v>
@@ -8304,7 +8304,7 @@
         <v>36</v>
       </c>
       <c r="CO14" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP14" t="s">
         <v>36</v>
@@ -8771,7 +8771,7 @@
         <v>36</v>
       </c>
       <c r="CO15" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP15" t="s">
         <v>36</v>
@@ -9238,7 +9238,7 @@
         <v>36</v>
       </c>
       <c r="CO16" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP16" t="s">
         <v>36</v>
@@ -9705,7 +9705,7 @@
         <v>36</v>
       </c>
       <c r="CO17" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP17" t="s">
         <v>36</v>
@@ -10172,7 +10172,7 @@
         <v>36</v>
       </c>
       <c r="CO18" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="CP18" t="s">
         <v>36</v>
@@ -10639,7 +10639,7 @@
         <v>36</v>
       </c>
       <c r="CO19" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP19" t="s">
         <v>36</v>
@@ -11106,7 +11106,7 @@
         <v>36</v>
       </c>
       <c r="CO20" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP20" t="s">
         <v>36</v>
@@ -11573,7 +11573,7 @@
         <v>36</v>
       </c>
       <c r="CO21" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP21" t="s">
         <v>36</v>
@@ -12040,7 +12040,7 @@
         <v>36</v>
       </c>
       <c r="CO22" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP22" t="s">
         <v>36</v>
@@ -12507,7 +12507,7 @@
         <v>36</v>
       </c>
       <c r="CO23" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP23" t="s">
         <v>36</v>
@@ -12974,7 +12974,7 @@
         <v>36</v>
       </c>
       <c r="CO24" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP24" t="s">
         <v>36</v>
@@ -13441,7 +13441,7 @@
         <v>36</v>
       </c>
       <c r="CO25" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP25" t="s">
         <v>36</v>
@@ -13908,7 +13908,7 @@
         <v>36</v>
       </c>
       <c r="CO26" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP26" t="s">
         <v>36</v>
@@ -14375,7 +14375,7 @@
         <v>36</v>
       </c>
       <c r="CO27" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP27" t="s">
         <v>36</v>
@@ -14842,7 +14842,7 @@
         <v>36</v>
       </c>
       <c r="CO28" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP28" t="s">
         <v>36</v>
@@ -15309,7 +15309,7 @@
         <v>36</v>
       </c>
       <c r="CO29" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP29" t="s">
         <v>36</v>
@@ -15776,7 +15776,7 @@
         <v>36</v>
       </c>
       <c r="CO30" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP30" t="s">
         <v>36</v>
@@ -16243,7 +16243,7 @@
         <v>36</v>
       </c>
       <c r="CO31" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP31" t="s">
         <v>36</v>
@@ -16710,7 +16710,7 @@
         <v>36</v>
       </c>
       <c r="CO32" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP32" t="s">
         <v>36</v>
@@ -17177,7 +17177,7 @@
         <v>36</v>
       </c>
       <c r="CO33" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP33" t="s">
         <v>36</v>
@@ -17644,7 +17644,7 @@
         <v>36</v>
       </c>
       <c r="CO34" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP34" t="s">
         <v>36</v>
@@ -18111,7 +18111,7 @@
         <v>36</v>
       </c>
       <c r="CO35" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP35" t="s">
         <v>36</v>
@@ -18578,7 +18578,7 @@
         <v>36</v>
       </c>
       <c r="CO36" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP36" t="s">
         <v>36</v>
@@ -19045,7 +19045,7 @@
         <v>36</v>
       </c>
       <c r="CO37" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP37" t="s">
         <v>36</v>
@@ -19512,7 +19512,7 @@
         <v>36</v>
       </c>
       <c r="CO38" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP38" t="s">
         <v>36</v>
@@ -19979,7 +19979,7 @@
         <v>36</v>
       </c>
       <c r="CO39" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP39" t="s">
         <v>36</v>
@@ -20446,7 +20446,7 @@
         <v>36</v>
       </c>
       <c r="CO40" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP40" t="s">
         <v>36</v>
@@ -20913,7 +20913,7 @@
         <v>36</v>
       </c>
       <c r="CO41" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="CP41" t="s">
         <v>36</v>
@@ -21380,7 +21380,7 @@
         <v>36</v>
       </c>
       <c r="CO42" t="s">
-        <v>439</v>
+        <v>36</v>
       </c>
       <c r="CP42" t="s">
         <v>36</v>

</xml_diff>